<commit_message>
canteen:report generation timeout increased
</commit_message>
<xml_diff>
--- a/canteen/controllers/thisMonthReport.xlsx
+++ b/canteen/controllers/thisMonthReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Order ID</t>
   </si>
@@ -28,6 +28,21 @@
     <t>Payment Mode</t>
   </si>
   <si>
+    <t>63dfe8107771d34b50ec1f77</t>
+  </si>
+  <si>
+    <t>het</t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>KOT</t>
+  </si>
+  <si>
     <t>63e07eaf09901c4fc0bb277e</t>
   </si>
   <si>
@@ -43,19 +58,16 @@
     <t>CASH</t>
   </si>
   <si>
-    <t>63dfe8107771d34b50ec1f77</t>
-  </si>
-  <si>
-    <t>het</t>
-  </si>
-  <si>
-    <t>360</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>KOT</t>
+    <t>63e07e8109901c4fc0bb2751</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>63e07f3509901c4fc0bb27fa</t>
+  </si>
+  <si>
+    <t>280</t>
   </si>
   <si>
     <t>63e0b01b09901c4fc0bb2877</t>
@@ -64,18 +76,6 @@
     <t>300</t>
   </si>
   <si>
-    <t>63e07e8109901c4fc0bb2751</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>63e07f3509901c4fc0bb27fa</t>
-  </si>
-  <si>
-    <t>280</t>
-  </si>
-  <si>
     <t>63e1d5998db3f87bb229b9f2</t>
   </si>
   <si>
@@ -88,37 +88,52 @@
     <t>63e1d7198db3f87bb229bb25</t>
   </si>
   <si>
+    <t>63e1ffe22c5b1158741302ca</t>
+  </si>
+  <si>
+    <t>63e203232c5b115874130468</t>
+  </si>
+  <si>
+    <t>610</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>63e22be88db3f87bb229bb74</t>
   </si>
   <si>
     <t>230</t>
   </si>
   <si>
-    <t>63e1ffe22c5b1158741302ca</t>
-  </si>
-  <si>
-    <t>63e203232c5b115874130468</t>
-  </si>
-  <si>
-    <t>610</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>63e22d478db3f87bb229bc52</t>
+  </si>
+  <si>
+    <t>Ayushi</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>63e22f0f8db3f87bb229bf35</t>
   </si>
   <si>
-    <t>Ayushi</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
-    <t>63e22d478db3f87bb229bc52</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>63e22f5e8db3f87bb229bf95</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>63e22f708db3f87bb229c035</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>63e22f938db3f87bb229c08a</t>
@@ -130,21 +145,6 @@
     <t>13</t>
   </si>
   <si>
-    <t>63e22f708db3f87bb229c035</t>
-  </si>
-  <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>63e22f5e8db3f87bb229bf95</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
     <t>63e3b550b7feef2bc93c71a7</t>
   </si>
   <si>
@@ -166,42 +166,42 @@
     <t>200</t>
   </si>
   <si>
+    <t>63e4882611e4eb3328e964db</t>
+  </si>
+  <si>
+    <t>kandarp shah</t>
+  </si>
+  <si>
     <t>63e486d511e4eb3328e96458</t>
   </si>
   <si>
-    <t>kandarp shah</t>
-  </si>
-  <si>
     <t>1080</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>63e4882611e4eb3328e964db</t>
-  </si>
-  <si>
     <t>63e48b7311e4eb3328e965ad</t>
   </si>
   <si>
+    <t>63e4926111e4eb3328e96993</t>
+  </si>
+  <si>
     <t>63e5100c05861c20302bf08d</t>
   </si>
   <si>
-    <t>63e4926111e4eb3328e96993</t>
-  </si>
-  <si>
     <t>63e51b274bde7a495d8ec15e</t>
   </si>
   <si>
+    <t>63e53cf2bc76bd300c9dc05c</t>
+  </si>
+  <si>
     <t>63e551ac4bde7a495d8ec7d5</t>
   </si>
   <si>
     <t>63e552041159a16eb41ee78a</t>
   </si>
   <si>
-    <t>63e53cf2bc76bd300c9dc05c</t>
-  </si>
-  <si>
     <t>63e55cae4bde7a495d8ec7fe</t>
   </si>
   <si>
@@ -223,15 +223,15 @@
     <t>ONLINE</t>
   </si>
   <si>
+    <t>63e563a315af2b3b20982b1a</t>
+  </si>
+  <si>
     <t>63e565164bde7a495d8ee7ea</t>
   </si>
   <si>
     <t>220</t>
   </si>
   <si>
-    <t>63e563a315af2b3b20982b1a</t>
-  </si>
-  <si>
     <t>63e565688dc3223c9284e885</t>
   </si>
   <si>
@@ -247,19 +247,31 @@
     <t>63e61a35a743527e2a29a20d</t>
   </si>
   <si>
+    <t>63e650aca743527e2a29a3b2</t>
+  </si>
+  <si>
     <t>63e6504ca743527e2a29a373</t>
   </si>
   <si>
     <t>140</t>
   </si>
   <si>
-    <t>63e650aca743527e2a29a3b2</t>
-  </si>
-  <si>
     <t>63e654a6fbb9f7b872e24a14</t>
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>63e6837804b4c646f8cff8ef</t>
+  </si>
+  <si>
+    <t>63e691d11ecee3b620a9c9be</t>
+  </si>
+  <si>
+    <t>3600</t>
+  </si>
+  <si>
+    <t>63e6846155206a37cc50b08b</t>
   </si>
 </sst>
 </file>
@@ -305,7 +317,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -367,16 +379,16 @@
         <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -384,16 +396,16 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -401,16 +413,16 @@
         <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -427,7 +439,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -438,13 +450,13 @@
         <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -452,13 +464,13 @@
         <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>14</v>
@@ -466,33 +478,33 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>9</v>
@@ -509,10 +521,10 @@
         <v>33</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -526,10 +538,10 @@
         <v>35</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -543,44 +555,44 @@
         <v>37</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="E15" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="E16" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -597,7 +609,7 @@
         <v>23</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -614,7 +626,7 @@
         <v>48</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -631,7 +643,7 @@
         <v>23</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -642,30 +654,30 @@
         <v>52</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -682,7 +694,7 @@
         <v>23</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -690,16 +702,16 @@
         <v>57</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -707,16 +719,16 @@
         <v>58</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -727,13 +739,13 @@
         <v>22</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -750,7 +762,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -758,13 +770,13 @@
         <v>61</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>9</v>
@@ -775,13 +787,13 @@
         <v>62</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>14</v>
@@ -798,10 +810,10 @@
         <v>64</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -812,13 +824,13 @@
         <v>22</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -832,10 +844,10 @@
         <v>67</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -860,33 +872,33 @@
         <v>70</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D34" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -917,10 +929,10 @@
         <v>76</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -931,13 +943,13 @@
         <v>32</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -945,33 +957,33 @@
         <v>78</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="D39" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -979,15 +991,66 @@
         <v>81</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>82</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E40" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>